<commit_message>
Update ANSI standard title blocks border lines and paper sizes.xlsx
</commit_message>
<xml_diff>
--- a/2D Drawings/ANSI standard title blocks border lines and paper sizes.xlsx
+++ b/2D Drawings/ANSI standard title blocks border lines and paper sizes.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B62FE98E-307F-40B0-8598-54F6390F469E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F41B434-4B81-427F-8737-F5CA9D8E5746}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Standard Title Blocks borders " sheetId="1" r:id="rId1"/>
@@ -259,46 +259,46 @@
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -589,6 +589,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="3.140625" customWidth="1"/>
     <col min="2" max="2" width="21.5703125" customWidth="1"/>
     <col min="3" max="3" width="18.85546875" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" customWidth="1"/>
@@ -597,246 +598,246 @@
     <col min="7" max="7" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="1" spans="2:11" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="1" t="s">
+      <c r="F2" s="11"/>
+      <c r="G2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="3" t="s">
+      <c r="I2" s="11"/>
+      <c r="J2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="4"/>
+      <c r="K2" s="11"/>
     </row>
     <row r="3" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="5" t="s">
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="5" t="s">
+      <c r="G3" s="14"/>
+      <c r="H3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="2">
         <v>8.5</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="7">
         <v>11</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="2">
         <v>0.38</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="2">
         <v>0.25</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="2">
         <v>210</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="2">
         <v>8.27</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4" s="2">
         <v>297</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K4" s="2">
         <v>11.69</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="5">
         <v>11</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="3">
         <v>8.5</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="3">
         <v>0.25</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="3">
         <v>0.38</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="K5" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="5">
         <v>11</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="5">
         <v>17</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="3">
         <v>0.38</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="3">
         <v>0.62</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="3">
         <v>297</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="3">
         <v>11.69</v>
       </c>
-      <c r="J6" s="8">
+      <c r="J6" s="3">
         <v>420</v>
       </c>
-      <c r="K6" s="8">
+      <c r="K6" s="3">
         <v>16.54</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="5">
         <v>17</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="5">
         <v>22</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="3">
         <v>0.75</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="8">
         <v>0.5</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="3">
         <v>420</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="3">
         <v>16.54</v>
       </c>
-      <c r="J7" s="8">
+      <c r="J7" s="3">
         <v>594</v>
       </c>
-      <c r="K7" s="8">
+      <c r="K7" s="3">
         <v>23.39</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="5">
         <v>22</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="5">
         <v>34</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="8">
         <v>0.5</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="8">
         <v>1</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="3">
         <v>594</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I8" s="3">
         <v>23.39</v>
       </c>
-      <c r="J8" s="8">
+      <c r="J8" s="3">
         <v>841</v>
       </c>
-      <c r="K8" s="8">
+      <c r="K8" s="3">
         <v>33.11</v>
       </c>
     </row>
     <row r="9" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="6">
         <v>34</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="6">
         <v>44</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="9">
         <v>1</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="9">
         <v>0.5</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="4">
         <v>841</v>
       </c>
-      <c r="I9" s="9">
+      <c r="I9" s="4">
         <v>33.11</v>
       </c>
-      <c r="J9" s="9">
+      <c r="J9" s="4">
         <v>1189</v>
       </c>
-      <c r="K9" s="9">
+      <c r="K9" s="4">
         <v>46.11</v>
       </c>
     </row>

</xml_diff>